<commit_message>
update the code ideas
</commit_message>
<xml_diff>
--- a/resources/data.xlsx
+++ b/resources/data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25629"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\T1725\Desktop\FUZZY_AHP\resources\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8067FE9C-3BA5-47EB-8232-DF30722E09A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="17820" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="因素反馈" sheetId="1" r:id="rId1"/>
@@ -113,14 +119,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-  </numFmts>
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,345 +129,21 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
+      <sz val="9"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="33">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="9">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -475,317 +151,34 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
-    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
-    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
-    <cellStyle name="输入" xfId="3" builtinId="20"/>
-    <cellStyle name="货币" xfId="4" builtinId="4"/>
-    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
-    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
-    <cellStyle name="差" xfId="7" builtinId="27"/>
-    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
-    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
-    <cellStyle name="超链接" xfId="10" builtinId="8"/>
-    <cellStyle name="百分比" xfId="11" builtinId="5"/>
-    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
-    <cellStyle name="注释" xfId="13" builtinId="10"/>
-    <cellStyle name="60% - 强调文字颜色 2" xfId="14" builtinId="36"/>
-    <cellStyle name="标题 4" xfId="15" builtinId="19"/>
-    <cellStyle name="警告文本" xfId="16" builtinId="11"/>
-    <cellStyle name="标题" xfId="17" builtinId="15"/>
-    <cellStyle name="解释性文本" xfId="18" builtinId="53"/>
-    <cellStyle name="标题 1" xfId="19" builtinId="16"/>
-    <cellStyle name="标题 2" xfId="20" builtinId="17"/>
-    <cellStyle name="60% - 强调文字颜色 1" xfId="21" builtinId="32"/>
-    <cellStyle name="标题 3" xfId="22" builtinId="18"/>
-    <cellStyle name="60% - 强调文字颜色 4" xfId="23" builtinId="44"/>
-    <cellStyle name="输出" xfId="24" builtinId="21"/>
-    <cellStyle name="计算" xfId="25" builtinId="22"/>
-    <cellStyle name="检查单元格" xfId="26" builtinId="23"/>
-    <cellStyle name="20% - 强调文字颜色 6" xfId="27" builtinId="50"/>
-    <cellStyle name="强调文字颜色 2" xfId="28" builtinId="33"/>
-    <cellStyle name="链接单元格" xfId="29" builtinId="24"/>
-    <cellStyle name="汇总" xfId="30" builtinId="25"/>
-    <cellStyle name="好" xfId="31" builtinId="26"/>
-    <cellStyle name="适中" xfId="32" builtinId="28"/>
-    <cellStyle name="20% - 强调文字颜色 5" xfId="33" builtinId="46"/>
-    <cellStyle name="强调文字颜色 1" xfId="34" builtinId="29"/>
-    <cellStyle name="20% - 强调文字颜色 1" xfId="35" builtinId="30"/>
-    <cellStyle name="40% - 强调文字颜色 1" xfId="36" builtinId="31"/>
-    <cellStyle name="20% - 强调文字颜色 2" xfId="37" builtinId="34"/>
-    <cellStyle name="40% - 强调文字颜色 2" xfId="38" builtinId="35"/>
-    <cellStyle name="强调文字颜色 3" xfId="39" builtinId="37"/>
-    <cellStyle name="强调文字颜色 4" xfId="40" builtinId="41"/>
-    <cellStyle name="20% - 强调文字颜色 4" xfId="41" builtinId="42"/>
-    <cellStyle name="40% - 强调文字颜色 4" xfId="42" builtinId="43"/>
-    <cellStyle name="强调文字颜色 5" xfId="43" builtinId="45"/>
-    <cellStyle name="40% - 强调文字颜色 5" xfId="44" builtinId="47"/>
-    <cellStyle name="60% - 强调文字颜色 5" xfId="45" builtinId="48"/>
-    <cellStyle name="强调文字颜色 6" xfId="46" builtinId="49"/>
-    <cellStyle name="40% - 强调文字颜色 6" xfId="47" builtinId="51"/>
-    <cellStyle name="60% - 强调文字颜色 6" xfId="48" builtinId="52"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1043,24 +436,24 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.375" customWidth="1"/>
+    <col min="1" max="1" width="18.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1076,7 +469,7 @@
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2">
         <v>1</v>
@@ -1106,12 +499,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1125,7 +518,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:10">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1136,7 +529,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1147,7 +540,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1161,12 +554,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1177,7 +570,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1188,12 +581,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:10">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1201,7 +594,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1215,7 +608,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1229,7 +622,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1243,7 +636,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:10">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1254,12 +647,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1270,7 +663,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1292,26 +685,25 @@
     <mergeCell ref="B1:J1"/>
     <mergeCell ref="A1:A2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D63" sqref="D63"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelCol="6"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="15.75" customHeight="1" spans="1:7">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>19</v>
       </c>
@@ -1326,7 +718,7 @@
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" t="s">
@@ -1345,16 +737,13 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3"/>
-      <c r="D3"/>
-      <c r="E3"/>
       <c r="F3">
         <v>5</v>
       </c>
@@ -1362,14 +751,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1"/>
       <c r="B4" t="s">
         <v>9</v>
       </c>
-      <c r="C4"/>
-      <c r="D4"/>
-      <c r="E4"/>
       <c r="F4">
         <v>6</v>
       </c>
@@ -1377,20 +763,16 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1"/>
       <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5"/>
-      <c r="D5"/>
-      <c r="E5"/>
-      <c r="F5"/>
       <c r="G5">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1"/>
       <c r="B6" t="s">
         <v>12</v>
@@ -1402,12 +784,11 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
       <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="C7"/>
       <c r="D7">
         <v>4</v>
       </c>
@@ -1415,12 +796,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1"/>
       <c r="B8" t="s">
         <v>14</v>
       </c>
-      <c r="C8"/>
       <c r="D8">
         <v>4</v>
       </c>
@@ -1428,14 +808,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
       <c r="B9" t="s">
         <v>15</v>
       </c>
-      <c r="C9"/>
-      <c r="D9"/>
-      <c r="E9"/>
       <c r="F9">
         <v>6</v>
       </c>
@@ -1443,36 +820,29 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" t="s">
         <v>17</v>
       </c>
-      <c r="C10"/>
-      <c r="D10"/>
       <c r="E10">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" t="s">
         <v>18</v>
       </c>
-      <c r="C11"/>
-      <c r="D11"/>
       <c r="E11">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" t="s">
         <v>27</v>
       </c>
-      <c r="C12"/>
-      <c r="D12"/>
-      <c r="E12"/>
       <c r="F12">
         <v>4</v>
       </c>
@@ -1480,7 +850,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>28</v>
       </c>
@@ -1494,12 +864,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" t="s">
         <v>9</v>
       </c>
-      <c r="C14"/>
       <c r="D14">
         <v>5</v>
       </c>
@@ -1507,7 +876,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" t="s">
         <v>11</v>
@@ -1519,26 +888,20 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C16"/>
-      <c r="D16"/>
-      <c r="E16"/>
-      <c r="F16"/>
       <c r="G16">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:6">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" t="s">
         <v>13</v>
       </c>
-      <c r="C17"/>
-      <c r="D17"/>
       <c r="E17">
         <v>3</v>
       </c>
@@ -1546,13 +909,11 @@
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" t="s">
         <v>14</v>
       </c>
-      <c r="C18"/>
-      <c r="D18"/>
       <c r="E18">
         <v>2</v>
       </c>
@@ -1560,14 +921,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" t="s">
         <v>15</v>
       </c>
-      <c r="C19"/>
-      <c r="D19"/>
-      <c r="E19"/>
       <c r="F19">
         <v>7</v>
       </c>
@@ -1575,23 +933,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20"/>
-      <c r="D20"/>
       <c r="E20">
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:5">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21"/>
       <c r="D21">
         <v>1</v>
       </c>
@@ -1599,7 +954,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" t="s">
         <v>27</v>
@@ -1614,15 +969,13 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
         <v>29</v>
       </c>
       <c r="B23" t="s">
         <v>8</v>
       </c>
-      <c r="C23"/>
-      <c r="D23"/>
       <c r="E23">
         <v>4</v>
       </c>
@@ -1630,12 +983,11 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:5">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" t="s">
         <v>9</v>
       </c>
-      <c r="C24"/>
       <c r="D24">
         <v>5</v>
       </c>
@@ -1643,14 +995,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:7">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" t="s">
         <v>11</v>
       </c>
-      <c r="C25"/>
-      <c r="D25"/>
-      <c r="E25"/>
       <c r="F25">
         <v>4</v>
       </c>
@@ -1658,14 +1007,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:7">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" t="s">
         <v>12</v>
       </c>
-      <c r="C26"/>
-      <c r="D26"/>
-      <c r="E26"/>
       <c r="F26">
         <v>1</v>
       </c>
@@ -1673,14 +1019,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="27" spans="1:7">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" t="s">
         <v>13</v>
       </c>
-      <c r="C27"/>
-      <c r="D27"/>
-      <c r="E27"/>
       <c r="F27">
         <v>2</v>
       </c>
@@ -1688,14 +1031,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="28" spans="1:7">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" t="s">
         <v>14</v>
       </c>
-      <c r="C28"/>
-      <c r="D28"/>
-      <c r="E28"/>
       <c r="F28">
         <v>2</v>
       </c>
@@ -1703,7 +1043,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:5">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" t="s">
         <v>15</v>
@@ -1718,23 +1058,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:5">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" t="s">
         <v>17</v>
       </c>
-      <c r="C30"/>
-      <c r="D30"/>
       <c r="E30">
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="1:5">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" t="s">
         <v>18</v>
       </c>
-      <c r="C31"/>
       <c r="D31">
         <v>1</v>
       </c>
@@ -1742,25 +1079,22 @@
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:5">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" t="s">
         <v>27</v>
       </c>
-      <c r="C32"/>
-      <c r="D32"/>
       <c r="E32">
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B33" t="s">
         <v>8</v>
       </c>
-      <c r="C33"/>
       <c r="D33">
         <v>5</v>
       </c>
@@ -1768,12 +1102,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:5">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" t="s">
         <v>9</v>
       </c>
-      <c r="C34"/>
       <c r="D34">
         <v>5</v>
       </c>
@@ -1781,14 +1114,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" t="s">
         <v>11</v>
       </c>
-      <c r="C35"/>
-      <c r="D35"/>
-      <c r="E35"/>
       <c r="F35">
         <v>4</v>
       </c>
@@ -1796,14 +1126,11 @@
         <v>4</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" t="s">
         <v>12</v>
       </c>
-      <c r="C36"/>
-      <c r="D36"/>
-      <c r="E36"/>
       <c r="F36">
         <v>1</v>
       </c>
@@ -1811,14 +1138,11 @@
         <v>7</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" t="s">
         <v>13</v>
       </c>
-      <c r="C37"/>
-      <c r="D37"/>
-      <c r="E37"/>
       <c r="F37">
         <v>2</v>
       </c>
@@ -1826,14 +1150,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="38" spans="1:7">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" t="s">
         <v>14</v>
       </c>
-      <c r="C38"/>
-      <c r="D38"/>
-      <c r="E38"/>
       <c r="F38">
         <v>2</v>
       </c>
@@ -1841,13 +1162,11 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:7">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" t="s">
         <v>15</v>
       </c>
-      <c r="C39"/>
-      <c r="D39"/>
       <c r="E39">
         <v>2</v>
       </c>
@@ -1858,23 +1177,20 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:5">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" t="s">
         <v>17</v>
       </c>
-      <c r="C40"/>
-      <c r="D40"/>
       <c r="E40">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:5">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
       <c r="B41" t="s">
         <v>18</v>
       </c>
-      <c r="C41"/>
       <c r="D41">
         <v>1</v>
       </c>
@@ -1882,27 +1198,26 @@
         <v>7</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" s="2"/>
       <c r="B42" t="s">
         <v>27</v>
       </c>
-      <c r="C42"/>
-      <c r="D42"/>
       <c r="E42">
         <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="A33:A42"/>
+    <mergeCell ref="B1:B2"/>
     <mergeCell ref="C1:G1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="A3:A12"/>
     <mergeCell ref="A13:A22"/>
     <mergeCell ref="A23:A32"/>
-    <mergeCell ref="A33:A42"/>
-    <mergeCell ref="B1:B2"/>
   </mergeCells>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>